<commit_message>
Initial submission to Clutter.
</commit_message>
<xml_diff>
--- a/sqlpad/cache/Dq1RSaZyPWG1gGwC.xlsx
+++ b/sqlpad/cache/Dq1RSaZyPWG1gGwC.xlsx
@@ -372,7 +372,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C8"/>
+  <dimension ref="A1:C9"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
@@ -393,7 +393,7 @@
         <v>edit</v>
       </c>
       <c r="C2" t="str">
-        <v>144</v>
+        <v>3471</v>
       </c>
     </row>
     <row r="3">
@@ -404,7 +404,7 @@
         <v>edit</v>
       </c>
       <c r="C3" t="str">
-        <v>118</v>
+        <v>2973</v>
       </c>
     </row>
     <row r="4">
@@ -415,7 +415,7 @@
         <v>categorize</v>
       </c>
       <c r="C4" t="str">
-        <v>66</v>
+        <v>2161</v>
       </c>
     </row>
     <row r="5">
@@ -426,7 +426,7 @@
         <v>new</v>
       </c>
       <c r="C5" t="str">
-        <v>31</v>
+        <v>747</v>
       </c>
     </row>
     <row r="6">
@@ -437,7 +437,7 @@
         <v>log</v>
       </c>
       <c r="C6" t="str">
-        <v>16</v>
+        <v>355</v>
       </c>
     </row>
     <row r="7">
@@ -448,18 +448,29 @@
         <v>categorize</v>
       </c>
       <c r="C7" t="str">
-        <v>15</v>
+        <v>228</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="b">
+        <v>1</v>
+      </c>
+      <c r="B8" t="str">
+        <v>log</v>
+      </c>
+      <c r="C8" t="str">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="b">
         <v>0</v>
       </c>
-      <c r="B8" t="str">
+      <c r="B9" t="str">
         <v>new</v>
       </c>
-      <c r="C8" t="str">
-        <v>10</v>
+      <c r="C9" t="str">
+        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>